<commit_message>
Added Sample-WorkTime excel-file for tests. (TODO: Update/correct tests)
</commit_message>
<xml_diff>
--- a/src/test/resources/excelWorkTimeSupplierTestFile.xlsx
+++ b/src/test/resources/excelWorkTimeSupplierTestFile.xlsx
@@ -1568,7 +1568,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1636,7 +1636,7 @@
         <v>0.652777777777778</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="G3" s="19"/>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="F4" s="22" t="n">
         <f aca="false">IF(AND(ISNUMBER(F2), ISNUMBER(F3), F3 &gt; F2), F3-F2, IF(AND(ISNUMBER(F2), ISNUMBER(F3)), (F3+day) - F2, ""))</f>
-        <v>0.333333333333333</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="G4" s="22" t="str">
         <f aca="false">IF(AND(ISNUMBER(G2), ISNUMBER(G3), G3 &gt; G2), G3-G2, IF(AND(ISNUMBER(G2), ISNUMBER(G3)), (G3+day) - G2, ""))</f>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="H4" s="23" t="n">
         <f aca="false">IF(OR(ISNUMBER(C4), ISNUMBER(D4), ISNUMBER(E4), ISNUMBER(F4), ISNUMBER(G4)), SUM(C4:G4), "")</f>
-        <v>1.29166666666667</v>
+        <v>1.04166666666667</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,7 +1680,9 @@
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="F5" s="25" t="n">
+        <v>0.541666666666667</v>
+      </c>
       <c r="G5" s="26" t="n">
         <v>0.361111111111111</v>
       </c>
@@ -1693,7 +1695,9 @@
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="F6" s="28" t="n">
+        <v>0.833333333333333</v>
+      </c>
       <c r="G6" s="29" t="n">
         <v>0.673611111111111</v>
       </c>
@@ -1715,9 +1719,9 @@
         <f aca="false">IF(AND(ISNUMBER(E5), ISNUMBER(E6), E6 &gt; E5), E6-E5, IF(AND(ISNUMBER(E5), ISNUMBER(E6)), (E6+day) - E5, ""))</f>
         <v/>
       </c>
-      <c r="F7" s="31" t="str">
+      <c r="F7" s="31" t="n">
         <f aca="false">IF(AND(ISNUMBER(F5), ISNUMBER(F6), F6 &gt; F5), F6-F5, IF(AND(ISNUMBER(F5), ISNUMBER(F6)), (F6+day) - F5, ""))</f>
-        <v/>
+        <v>0.291666666666667</v>
       </c>
       <c r="G7" s="32" t="n">
         <f aca="false">IF(AND(ISNUMBER(G5), ISNUMBER(G6), G6 &gt; G5), G6-G5, IF(AND(ISNUMBER(G5), ISNUMBER(G6)), (G6+day) - G5, ""))</f>
@@ -1725,7 +1729,7 @@
       </c>
       <c r="H7" s="23" t="n">
         <f aca="false">IF(OR(ISNUMBER(C7), ISNUMBER(D7), ISNUMBER(E7), ISNUMBER(F7), ISNUMBER(G7)), SUM(C7:G7), "")</f>
-        <v>0.3125</v>
+        <v>0.604166666666667</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,7 +1751,7 @@
       </c>
       <c r="F8" s="35" t="n">
         <f aca="false">IF(SUM(F4,F7) &gt; 0, SUM(F4,F7)*24, "")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" s="36" t="n">
         <f aca="false">IF(SUM(G4,G7) &gt; 0, SUM(G4,G7)*24, "")</f>
@@ -1755,7 +1759,7 @@
       </c>
       <c r="H8" s="37" t="n">
         <f aca="false">IF(OR(ISNUMBER(C8), ISNUMBER(D8), ISNUMBER(E8), ISNUMBER(F8)), SUM(C8:G8), "")</f>
-        <v>38.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1777,7 +1781,7 @@
       </c>
       <c r="F9" s="40" t="n">
         <f aca="false">IF(ISNUMBER(F8),IF(F8 &gt;= 9, TIME(0,45,0), IF(F8 &gt;= 6, TIME(0,30,0), TIME(0,0,0))), "")</f>
-        <v>0.0208333333333333</v>
+        <v>0.03125</v>
       </c>
       <c r="G9" s="41" t="n">
         <f aca="false">IF(ISNUMBER(G8),IF(G8 &gt;= 9, TIME(0,45,0), IF(G8 &gt;= 6, TIME(0,30,0), TIME(0,0,0))), "")</f>
@@ -1785,7 +1789,7 @@
       </c>
       <c r="H9" s="42" t="n">
         <f aca="false">IF(OR(ISNUMBER(C9), ISNUMBER(D9), ISNUMBER(E9), ISNUMBER(F9)), SUM(C9:G9), "")</f>
-        <v>0.104166666666667</v>
+        <v>0.114583333333333</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,7 +1811,7 @@
       </c>
       <c r="F10" s="45" t="n">
         <f aca="false">IF(AND(ISNUMBER(F8),ISNUMBER(F9)), (F8-(F9*24)), "")</f>
-        <v>7.5</v>
+        <v>8.25</v>
       </c>
       <c r="G10" s="46" t="n">
         <f aca="false">IF(AND(ISNUMBER(G8),ISNUMBER(G9)), (G8-(G9*24)), "")</f>
@@ -1815,7 +1819,7 @@
       </c>
       <c r="H10" s="47" t="n">
         <f aca="false">IF(OR(ISNUMBER(C10), ISNUMBER(D10), ISNUMBER(E10), ISNUMBER(F10)), SUM(C10:G10), "")</f>
-        <v>36</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>